<commit_message>
Fixed Some Params Issues
</commit_message>
<xml_diff>
--- a/paramData Excels/Q0019.xlsx
+++ b/paramData Excels/Q0019.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0A7BA79-192F-4440-8993-05561DF9A760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +105,6 @@
     <t>FreqFactor</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>P0050</t>
   </si>
   <si>
@@ -122,13 +118,16 @@
   </si>
   <si>
     <t>Factor based on Frequency</t>
+  </si>
+  <si>
+    <t>[0]string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,9 +204,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +244,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -279,7 +278,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -314,10 +312,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,14 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2:AA3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="10" max="10" width="37.77734375" customWidth="1"/>
@@ -506,7 +503,7 @@
     <col min="27" max="27" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -582,7 +579,7 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
@@ -603,22 +600,22 @@
         <v>23</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
         <v>28</v>
       </c>
       <c r="S2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27">
       <c r="C3">
         <v>2</v>
       </c>
@@ -644,7 +641,7 @@
         <v>22</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA3" s="2"/>
     </row>
@@ -655,24 +652,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>